<commit_message>
procx valor não encontrado
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/6.Funcoes_Mercado/9.PROCX/1.PROCX.xlsx
+++ b/2.Excel/hands-on/6.Funcoes_Mercado/9.PROCX/1.PROCX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\6.Funcoes_Mercado\9.PROCX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2198980-60B7-4B6B-A876-D374A57C326D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB380545-9066-4805-9E50-E73633BD481A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11652" yWindow="108" windowWidth="11376" windowHeight="12792" xr2:uid="{90D394A7-0334-4363-9DA1-420D95C76B52}"/>
+    <workbookView xWindow="11652" yWindow="108" windowWidth="11376" windowHeight="12792" activeTab="1" xr2:uid="{90D394A7-0334-4363-9DA1-420D95C76B52}"/>
   </bookViews>
   <sheets>
     <sheet name="PROCX1" sheetId="2" r:id="rId1"/>
@@ -1526,7 +1526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1809EF98-FC10-4422-B0BD-9E97AD3F071B}">
   <dimension ref="A1:H309"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -3770,7 +3770,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D440E865-CE29-4B59-BFD7-1552AC890A9B}">
   <dimension ref="A1:H309"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3878,11 +3880,11 @@
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H5" s="2" t="str">
         <f>_xlfn.XLOOKUP(G5,B:B,E:E,_xlfn.XLOOKUP(G5,C:C,E:E,"Não encontrado"))</f>
-        <v>Delta</v>
+        <v>Beta</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>